<commit_message>
Release of first public demo/User Manual, and Planing Docs
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Bugs.xlsx
+++ b/01_ProjectPlanning/Bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Bug</t>
   </si>
@@ -119,12 +119,27 @@
   </si>
   <si>
     <t>Ckecken ob Gameobject schon existiert</t>
+  </si>
+  <si>
+    <t>Enemy Healthbar BUG</t>
+  </si>
+  <si>
+    <t>Balken ist teilweise kurz wenn man draufschlägt, steigt dann rapide an und decreast auf den eigentlichen Wert</t>
+  </si>
+  <si>
+    <t>Stoney_Dialoge</t>
+  </si>
+  <si>
+    <t>Dialoge wird öfters gestartet</t>
+  </si>
+  <si>
+    <t>vermutlich CoRoutine mehrfach gestartet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,9 +233,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +273,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -330,7 +345,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -507,7 +522,7 @@
   <dimension ref="A2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +679,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -696,10 +711,16 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
@@ -718,9 +739,15 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>

</xml_diff>